<commit_message>
feat,test(all): add a PathController, a Path model, modify the tests to fit the new MVC architecture
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_colgetpartofstr.xlsx
+++ b/fichiers_xls/test_colgetpartofstr.xlsx
@@ -344,14 +344,14 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="947" max="1016"/>
-    <col width="11.53" customWidth="1" style="2" min="16377" max="16384"/>
+    <col width="11.52" customWidth="1" style="2" min="932" max="1001"/>
+    <col width="11.53" customWidth="1" style="2" min="16362" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
@@ -561,7 +561,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
factor(tests): write classes to factor first two tests
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_colgetpartofstr.xlsx
+++ b/fichiers_xls/test_colgetpartofstr.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille2" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="expected" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="expected2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlfn_T_TEST" hidden="0" function="0" vbProcedure="0">NA()</definedName>
@@ -344,14 +345,14 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="B1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="930" max="999"/>
-    <col width="11.53" customWidth="1" style="2" min="16360" max="16384"/>
+    <col width="11.52" customWidth="1" style="2" min="927" max="996"/>
+    <col width="11.53" customWidth="1" style="2" min="16357" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
@@ -558,16 +559,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="954" max="1023"/>
-    <col width="11.53" customWidth="1" style="2" min="16384" max="16384"/>
+    <col width="11.52" customWidth="1" style="2" min="953" max="1022"/>
+    <col width="11.53" customWidth="1" style="2" min="16383" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
@@ -620,11 +621,6 @@
           <t>Congruent1;o;.jpg</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
@@ -653,11 +649,6 @@
           <t>Incongruent1;n.jpg</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>n.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="3">
       <c r="A4" s="2" t="n"/>
@@ -681,11 +672,6 @@
           <t>Congruent2;o.jpg</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>o.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="3">
       <c r="A5" s="2" t="n"/>
@@ -709,11 +695,6 @@
           <t>congruent3;n.jpg</t>
         </is>
       </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>n.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="3">
       <c r="B6" s="2" t="inlineStr">
@@ -741,11 +722,6 @@
           <t>Congruent5;o.jpg</t>
         </is>
       </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>o.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="3">
       <c r="B7" s="2" t="inlineStr">
@@ -768,11 +744,6 @@
           <t>d1_o;.jpg</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
-        <is>
-          <t>.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="3">
       <c r="B8" s="2" t="inlineStr">
@@ -795,11 +766,6 @@
           <t>congruent1;_o.jpg</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>_o.jpg</t>
-        </is>
-      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="3">
       <c r="B9" s="2" t="inlineStr">
@@ -827,7 +793,258 @@
           <t>Neutre1;2_n.jpg</t>
         </is>
       </c>
-      <c r="G9" s="2" t="inlineStr">
+    </row>
+    <row r="1048576" ht="12.75" customHeight="1" s="3"/>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col width="11.52" customWidth="1" style="2" min="953" max="1022"/>
+    <col width="11.53" customWidth="1" style="2" min="16383" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75" customHeight="1" s="3">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Evaluatisme</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Absolutisme</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Multiplisme</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Colonne de(s) maximum(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.75" customHeight="1" s="3">
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>prime</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>congruent1_o.jpg</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>prime_congruent</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Congruent1;o;.jpg</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="3">
+      <c r="A3" s="2" t="n"/>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>probe</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>incongruent1_n.jpg</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>probe_incongruent</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Incongruent1;n.jpg</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>n.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="3">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>qfqfq</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>congruent2_o.jpg</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Congruent2;o.jpg</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>o.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="3">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>qvfqf</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>congruent3_n.jpg</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>congruent3;n.jpg</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>n.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="3">
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>probe</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>congruent5_o.jpg</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>probe_congruent</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Congruent5;o.jpg</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>o.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="3">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>pqfqf</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>d1_o.jpg</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>d1_o;.jpg</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="3">
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Prime</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>congruent1_o.jpg</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>congruent1;_o.jpg</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>_o.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="3">
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>prime</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>neutre12_n.jpg</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>prime_neutre</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Neutre1;2_n.jpg</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
         <is>
           <t>2_n.jpg</t>
         </is>

</xml_diff>